<commit_message>
changed spatial, subdomain description
</commit_message>
<xml_diff>
--- a/docs/EPOS_DCAT-AP_Vocabulary_and_Specification.xlsx
+++ b/docs/EPOS_DCAT-AP_Vocabulary_and_Specification.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="509">
   <si>
     <t>Unique Resource Identifier</t>
   </si>
@@ -1495,9 +1495,6 @@
   </si>
   <si>
     <t>This property contains the main identifier for Person. May be *ORCID for Persons; *Mailto: Literals like mailto:support@institution</t>
-  </si>
-  <si>
-    <t>This property refers to a geographical area related to the data we provide.It's espressed as a poliygon and supports multiple polygons when the data comes from different regions.. Skip elevation when the value is  0.</t>
   </si>
   <si>
     <r>
@@ -1587,6 +1584,12 @@
   </si>
   <si>
     <t>This property refers to the organisation responsible to publish the WebService.</t>
+  </si>
+  <si>
+    <t>This property refers to the subdomain of resource</t>
+  </si>
+  <si>
+    <t>This property refers to a geographical area related to the data we provide.It's espressed as a poliygon .Skip elevation when the value is  0.</t>
   </si>
 </sst>
 </file>
@@ -3991,10 +3994,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4007,6 +4022,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4025,19 +4041,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="107" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="98" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="112" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4063,6 +4066,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4092,18 +4107,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4589,10 +4592,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="357" t="s">
+      <c r="A13" s="361" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="359" t="s">
+      <c r="B13" s="363" t="s">
         <v>130</v>
       </c>
       <c r="C13" s="195" t="s">
@@ -4601,20 +4604,20 @@
       <c r="D13" s="196" t="s">
         <v>372</v>
       </c>
-      <c r="E13" s="361" t="s">
+      <c r="E13" s="365" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="358"/>
-      <c r="B14" s="360"/>
+      <c r="A14" s="367"/>
+      <c r="B14" s="364"/>
       <c r="C14" s="195" t="s">
         <v>370</v>
       </c>
       <c r="D14" s="196" t="s">
         <v>372</v>
       </c>
-      <c r="E14" s="362"/>
+      <c r="E14" s="366"/>
     </row>
     <row r="15" spans="1:5" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A15" s="205" t="s">
@@ -4702,10 +4705,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="367" t="s">
+      <c r="A20" s="372" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="365" t="s">
+      <c r="B20" s="370" t="s">
         <v>241</v>
       </c>
       <c r="C20" s="202" t="s">
@@ -4719,16 +4722,16 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="368"/>
-      <c r="B21" s="369"/>
+      <c r="A21" s="373"/>
+      <c r="B21" s="374"/>
       <c r="C21" s="355" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D21" s="200" t="s">
         <v>374</v>
       </c>
       <c r="E21" s="356" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.95" x14ac:dyDescent="0.2">
@@ -4766,10 +4769,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="363" t="s">
+      <c r="A24" s="368" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="365" t="s">
+      <c r="B24" s="370" t="s">
         <v>152</v>
       </c>
       <c r="C24" s="198" t="s">
@@ -4783,8 +4786,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="364"/>
-      <c r="B25" s="366"/>
+      <c r="A25" s="369"/>
+      <c r="B25" s="371"/>
       <c r="C25" s="198" t="s">
         <v>374</v>
       </c>
@@ -4796,10 +4799,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="357" t="s">
+      <c r="A26" s="361" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="359" t="s">
+      <c r="B26" s="363" t="s">
         <v>315</v>
       </c>
       <c r="C26" s="198" t="s">
@@ -4808,20 +4811,20 @@
       <c r="D26" s="200" t="s">
         <v>374</v>
       </c>
-      <c r="E26" s="361" t="s">
+      <c r="E26" s="365" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="374"/>
-      <c r="B27" s="360"/>
+      <c r="A27" s="362"/>
+      <c r="B27" s="364"/>
       <c r="C27" s="198" t="s">
         <v>162</v>
       </c>
       <c r="D27" s="203" t="s">
         <v>374</v>
       </c>
-      <c r="E27" s="362"/>
+      <c r="E27" s="366"/>
     </row>
     <row r="28" spans="1:5" ht="15.95" x14ac:dyDescent="0.2">
       <c r="A28" s="208" t="s">
@@ -4961,10 +4964,10 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="372" t="s">
+      <c r="A38" s="359" t="s">
         <v>408</v>
       </c>
-      <c r="B38" s="370" t="s">
+      <c r="B38" s="357" t="s">
         <v>398</v>
       </c>
       <c r="C38" s="258" t="s">
@@ -4976,8 +4979,8 @@
       <c r="E38" s="259"/>
     </row>
     <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="373"/>
-      <c r="B39" s="371"/>
+      <c r="A39" s="360"/>
+      <c r="B39" s="358"/>
       <c r="C39" s="213" t="s">
         <v>370</v>
       </c>
@@ -4988,11 +4991,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="E26:E27"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="E13:E14"/>
@@ -5000,6 +4998,11 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="E26:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5389,7 +5392,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E4" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F4" s="376"/>
       <c r="G4" s="377"/>
@@ -5408,7 +5411,7 @@
         <v>194</v>
       </c>
       <c r="E5" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F5" s="337" t="s">
         <v>413</v>
@@ -6007,7 +6010,7 @@
         <v>404</v>
       </c>
       <c r="I27" s="257" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.95" x14ac:dyDescent="0.2">
@@ -6030,7 +6033,7 @@
         <v>404</v>
       </c>
       <c r="I28" s="257" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -6053,7 +6056,7 @@
         <v>405</v>
       </c>
       <c r="I29" s="253" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -6536,8 +6539,8 @@
   </sheetPr>
   <dimension ref="A1:I224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6583,7 +6586,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E4" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F4" s="376"/>
       <c r="G4" s="377"/>
@@ -6602,7 +6605,7 @@
         <v>474</v>
       </c>
       <c r="E5" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F5" s="337" t="s">
         <v>413</v>
@@ -6796,7 +6799,7 @@
         <v>131</v>
       </c>
       <c r="B12" s="226" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C12" s="225" t="s">
         <v>370</v>
@@ -6871,7 +6874,7 @@
         <v>405</v>
       </c>
       <c r="I14" s="257" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -6900,7 +6903,7 @@
         <v>405</v>
       </c>
       <c r="I15" s="346" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6929,7 +6932,7 @@
         <v>405</v>
       </c>
       <c r="I16" s="346" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7016,7 +7019,7 @@
         <v>404</v>
       </c>
       <c r="I19" s="257" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.95" x14ac:dyDescent="0.2">
@@ -7039,7 +7042,7 @@
         <v>404</v>
       </c>
       <c r="I20" s="257" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.95" x14ac:dyDescent="0.2">
@@ -7062,7 +7065,7 @@
         <v>404</v>
       </c>
       <c r="I21" s="257" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7091,7 +7094,7 @@
         <v>404</v>
       </c>
       <c r="I22" s="257" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7154,10 +7157,10 @@
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="243" t="s">
+        <v>493</v>
+      </c>
+      <c r="B25" s="223" t="s">
         <v>494</v>
-      </c>
-      <c r="B25" s="223" t="s">
-        <v>495</v>
       </c>
       <c r="C25" s="225" t="s">
         <v>370</v>
@@ -7172,15 +7175,15 @@
         <v>407</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="243" t="s">
+        <v>490</v>
+      </c>
+      <c r="B26" s="223" t="s">
         <v>491</v>
-      </c>
-      <c r="B26" s="223" t="s">
-        <v>492</v>
       </c>
       <c r="C26" s="225" t="s">
         <v>370</v>
@@ -7195,7 +7198,7 @@
         <v>405</v>
       </c>
       <c r="I26" s="346" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -7291,7 +7294,7 @@
         <v>404</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -7316,7 +7319,7 @@
         <v>407</v>
       </c>
       <c r="I31" s="52" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -7339,7 +7342,7 @@
         <v>405</v>
       </c>
       <c r="I32" s="52" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -7362,7 +7365,7 @@
         <v>405</v>
       </c>
       <c r="I33" s="52" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9333,22 +9336,22 @@
       <c r="A1" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="387" t="s">
+      <c r="B1" s="391" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="387"/>
-      <c r="D1" s="388"/>
+      <c r="C1" s="391"/>
+      <c r="D1" s="392"/>
       <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="389" t="s">
+      <c r="B2" s="393" t="s">
         <v>371</v>
       </c>
-      <c r="C2" s="389"/>
-      <c r="D2" s="390"/>
+      <c r="C2" s="393"/>
+      <c r="D2" s="394"/>
       <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
@@ -9360,7 +9363,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E4" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F4" s="376"/>
       <c r="G4" s="377"/>
@@ -9379,7 +9382,7 @@
         <v>194</v>
       </c>
       <c r="E5" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F5" s="337" t="s">
         <v>413</v>
@@ -9427,13 +9430,13 @@
       <c r="A7" s="277" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="385" t="s">
+      <c r="B7" s="389" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="391" t="s">
+      <c r="C7" s="395" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="393" t="s">
+      <c r="D7" s="397" t="s">
         <v>202</v>
       </c>
       <c r="E7" s="246" t="s">
@@ -9445,10 +9448,10 @@
       <c r="G7" s="246" t="s">
         <v>416</v>
       </c>
-      <c r="H7" s="396" t="s">
+      <c r="H7" s="386" t="s">
         <v>404</v>
       </c>
-      <c r="I7" s="395" t="s">
+      <c r="I7" s="385" t="s">
         <v>289</v>
       </c>
     </row>
@@ -9456,9 +9459,9 @@
       <c r="A8" s="277" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="386"/>
-      <c r="C8" s="392"/>
-      <c r="D8" s="394"/>
+      <c r="B8" s="390"/>
+      <c r="C8" s="396"/>
+      <c r="D8" s="398"/>
       <c r="E8" s="246" t="s">
         <v>415</v>
       </c>
@@ -9468,8 +9471,8 @@
       <c r="G8" s="246" t="s">
         <v>416</v>
       </c>
-      <c r="H8" s="396"/>
-      <c r="I8" s="395"/>
+      <c r="H8" s="386"/>
+      <c r="I8" s="385"/>
     </row>
     <row r="9" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="277" t="s">
@@ -9598,13 +9601,13 @@
       <c r="D13" s="157" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="397" t="s">
+      <c r="E13" s="387" t="s">
         <v>415</v>
       </c>
-      <c r="F13" s="397">
+      <c r="F13" s="387">
         <v>128</v>
       </c>
-      <c r="G13" s="397" t="s">
+      <c r="G13" s="387" t="s">
         <v>420</v>
       </c>
       <c r="H13" s="228" t="s">
@@ -9627,9 +9630,9 @@
       <c r="D14" s="157" t="s">
         <v>203</v>
       </c>
-      <c r="E14" s="397"/>
-      <c r="F14" s="397"/>
-      <c r="G14" s="397"/>
+      <c r="E14" s="387"/>
+      <c r="F14" s="387"/>
+      <c r="G14" s="387"/>
       <c r="H14" s="228" t="s">
         <v>405</v>
       </c>
@@ -9650,9 +9653,9 @@
       <c r="D15" s="158" t="s">
         <v>203</v>
       </c>
-      <c r="E15" s="398"/>
-      <c r="F15" s="398"/>
-      <c r="G15" s="398"/>
+      <c r="E15" s="388"/>
+      <c r="F15" s="388"/>
+      <c r="G15" s="388"/>
       <c r="H15" s="237" t="s">
         <v>405</v>
       </c>
@@ -9669,17 +9672,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E13:E15"/>
     <mergeCell ref="F13:F15"/>
     <mergeCell ref="G13:G15"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9736,7 +9739,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E4" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F4" s="376"/>
       <c r="G4" s="377"/>
@@ -9755,7 +9758,7 @@
         <v>194</v>
       </c>
       <c r="E5" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F5" s="337" t="s">
         <v>413</v>
@@ -10329,7 +10332,7 @@
     <row r="3" spans="1:11" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8"/>
       <c r="E3" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F3" s="376"/>
       <c r="G3" s="377"/>
@@ -10348,7 +10351,7 @@
         <v>194</v>
       </c>
       <c r="E4" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F4" s="337" t="s">
         <v>413</v>
@@ -10617,7 +10620,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F3" s="376"/>
       <c r="G3" s="377"/>
@@ -10638,7 +10641,7 @@
         <v>194</v>
       </c>
       <c r="E4" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F4" s="337" t="s">
         <v>413</v>
@@ -10993,11 +10996,11 @@
       <c r="A2" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="389" t="s">
+      <c r="B2" s="393" t="s">
         <v>336</v>
       </c>
-      <c r="C2" s="389"/>
-      <c r="D2" s="389"/>
+      <c r="C2" s="393"/>
+      <c r="D2" s="393"/>
       <c r="E2" s="44"/>
       <c r="F2" s="8"/>
       <c r="H2"/>
@@ -11017,7 +11020,7 @@
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F4" s="376"/>
       <c r="G4" s="377"/>
@@ -11038,7 +11041,7 @@
         <v>194</v>
       </c>
       <c r="E5" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F5" s="337" t="s">
         <v>413</v>
@@ -11986,7 +11989,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="375" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F3" s="376"/>
       <c r="G3" s="377"/>
@@ -12006,7 +12009,7 @@
         <v>194</v>
       </c>
       <c r="E4" s="336" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F4" s="337" t="s">
         <v>413</v>

</xml_diff>